<commit_message>
Add logging flow and implment pending changes and fix database flow
</commit_message>
<xml_diff>
--- a/Data/Config_Dev.xlsx
+++ b/Data/Config_Dev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\REFProj\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5B275F-E9C5-409A-AF3A-1BC1DE90EE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3D84A8-A5B1-461A-A1B4-5DB18C5E678A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,7 +650,7 @@
   <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
fix the logging issue and exception handling
</commit_message>
<xml_diff>
--- a/Data/Config_Dev.xlsx
+++ b/Data/Config_Dev.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\REFProj\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\ReFrameworkTemplates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED77F59-18B6-4D35-B779-4B2A61C2C29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60AE3E9-E8E8-45AD-AFA5-3159FD095393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -219,16 +219,16 @@
     <t>StatusToProcess</t>
   </si>
   <si>
+    <t>OpenBrowserUrl</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/login</t>
+  </si>
+  <si>
+    <t>Data\Screenshots</t>
+  </si>
+  <si>
     <t>Data Source=10.20.30.82;Initial Catalog=CustomerDB;User Id=sql.user;Password=Asif@123;Encrypt=False</t>
-  </si>
-  <si>
-    <t>OpenBrowserUrl</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/login</t>
-  </si>
-  <si>
-    <t>Data\Screenshots</t>
   </si>
 </sst>
 </file>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -776,7 +776,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
@@ -805,10 +805,10 @@
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1797,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1871,7 +1871,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>

</xml_diff>